<commit_message>
remove extra sheet. Add consumer name warning message
</commit_message>
<xml_diff>
--- a/reporting_template.xlsx
+++ b/reporting_template.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\Git\CILs-first-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967F1EE8-7855-40E7-9D0A-154A2990650A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6852FE58-DF60-4021-AFBC-541783F2EDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="2" xr2:uid="{F0BE1F58-B81B-4224-92BC-96133C095D6B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{F0BE1F58-B81B-4224-92BC-96133C095D6B}"/>
   </bookViews>
   <sheets>
-    <sheet name="is" sheetId="1" r:id="rId1"/>
-    <sheet name="individual_services" sheetId="2" r:id="rId2"/>
-    <sheet name="Tables" sheetId="3" r:id="rId3"/>
+    <sheet name="individual_services" sheetId="2" r:id="rId1"/>
+    <sheet name="Tables" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,52 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
-  <si>
-    <t>contact_date</t>
-  </si>
-  <si>
-    <t>time_begun</t>
-  </si>
-  <si>
-    <t>time_ended</t>
-  </si>
-  <si>
-    <t>hours</t>
-  </si>
-  <si>
-    <t>consumer</t>
-  </si>
-  <si>
-    <t>service</t>
-  </si>
-  <si>
-    <t>priority_area</t>
-  </si>
-  <si>
-    <t>Brown, Erica</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Ongoing Support</t>
-  </si>
-  <si>
-    <t>funding_source</t>
-  </si>
-  <si>
-    <t>staff_comments</t>
-  </si>
-  <si>
-    <t>ir</t>
-  </si>
-  <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, ex mel possit alienum, eruditi alienum eu his. Facilis invidunt efficiendi et sea, odio iracundia est ea. Id vero legere deleniti est. Eu prodesset persequeris ius, tincidunt reprimique eu nam. Invidunt theophrastus eos at. Mel novum nemore eu</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>Hours</t>
   </si>
@@ -326,6 +280,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Youth Empower You</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -341,18 +304,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -412,21 +369,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -435,10 +386,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -493,6 +444,16 @@
   <autoFilter ref="D16:D42" xr:uid="{EE86F369-317F-418C-BA76-E9BC54EC67D1}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{B0028349-EE4D-4289-8632-16DBC40AA4DD}" name="Funding Source"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7909C059-2AB2-4C4D-A56E-6361791DCC5D}" name="Table6" displayName="Table6" ref="B34:B36" totalsRowShown="0">
+  <autoFilter ref="B34:B36" xr:uid="{7909C059-2AB2-4C4D-A56E-6361791DCC5D}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{4EBA9A07-62EF-416F-A801-06185FACC512}" name="IR"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -794,150 +755,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB40F976-7331-4B78-B22D-171CE55C2008}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475C1560-65C8-49F6-9B9A-F6715764C657}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.86328125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.06640625" style="1"/>
+    <col min="4" max="4" width="13.06640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.46484375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.53125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.86328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="46.86328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.06640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>44515</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475C1560-65C8-49F6-9B9A-F6715764C657}">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="18.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="5"/>
-    <col min="4" max="4" width="13.06640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.46484375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.53125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16.86328125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="46.86328125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="9.06640625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Spell check!" prompt="Please ensure both the last name and first name are spelled correctly and in the required format (Last, First)_x000a_" sqref="A2:A1048576" xr:uid="{C37A8EAA-4863-4C4F-9940-74929C156380}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{11BCFCDE-454A-4642-B56C-EB4EAADF1EEE}">
           <x14:formula1>
             <xm:f>Tables!$B$3:$B$32</xm:f>
@@ -950,18 +829,30 @@
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{BC393DBA-6318-40FF-B771-4B498D55A2CC}">
+          <x14:formula1>
+            <xm:f>Tables!$D$17:$D$42</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{B9C4133B-93F9-49DC-B258-9A5C2DAF76DC}">
+          <x14:formula1>
+            <xm:f>Tables!$B$35:$B$36</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D25536F-9C4B-4B66-A9D8-B0C5C74E4EE3}">
   <dimension ref="B2:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -972,303 +863,313 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
       <c r="D34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
       <c r="D35" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
       <c r="D36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D37" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D39" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D39" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.45">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D42" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add time and date data types to resolve import issues
</commit_message>
<xml_diff>
--- a/reporting_template.xlsx
+++ b/reporting_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\Git\CILs-first-bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matte/Git/CILs-first-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEB6A78-66BE-4EF8-9392-EACB77DF596A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E83772-0969-C24B-A7C2-3A99645AB41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{F0BE1F58-B81B-4224-92BC-96133C095D6B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22700" windowHeight="14600" xr2:uid="{F0BE1F58-B81B-4224-92BC-96133C095D6B}"/>
   </bookViews>
   <sheets>
     <sheet name="individual_services" sheetId="2" r:id="rId1"/>
@@ -295,6 +295,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -395,6 +398,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,24 +768,24 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1048548" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1048548" sqref="H1048548:H1048576"/>
+      <selection pane="bottomLeft" activeCell="B1048551" sqref="B1048551"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="1"/>
-    <col min="4" max="4" width="13.06640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.46484375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.53125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.86328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="46.86328125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.06640625" style="5"/>
+    <col min="2" max="2" width="16.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="13" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="46.83203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -861,13 +870,13 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="44.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -875,7 +884,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -883,7 +892,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -891,7 +900,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -899,7 +908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -907,7 +916,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -915,7 +924,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -923,7 +932,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -931,7 +940,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>39</v>
       </c>
@@ -939,7 +948,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -947,7 +956,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -955,7 +964,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -963,17 +972,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -981,7 +990,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -989,7 +998,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -997,7 +1006,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -1005,7 +1014,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>26</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>27</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>28</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>29</v>
       </c>
@@ -1037,7 +1046,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>30</v>
       </c>
@@ -1045,7 +1054,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>32</v>
       </c>
@@ -1061,7 +1070,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>33</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>34</v>
       </c>
@@ -1077,7 +1086,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -1085,7 +1094,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>36</v>
       </c>
@@ -1093,7 +1102,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>37</v>
       </c>
@@ -1101,7 +1110,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>38</v>
       </c>
@@ -1109,12 +1118,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>79</v>
       </c>
@@ -1122,7 +1131,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>80</v>
       </c>
@@ -1130,7 +1139,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>81</v>
       </c>
@@ -1138,32 +1147,32 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D39" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
remove individual services from reporting template
</commit_message>
<xml_diff>
--- a/reporting_template.xlsx
+++ b/reporting_template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matte/Git/CILs-first-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E83772-0969-C24B-A7C2-3A99645AB41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A671ED8F-63AE-024C-8AFA-F56A4E7E57C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22700" windowHeight="14600" xr2:uid="{F0BE1F58-B81B-4224-92BC-96133C095D6B}"/>
+    <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18880" activeTab="1" xr2:uid="{F0BE1F58-B81B-4224-92BC-96133C095D6B}"/>
   </bookViews>
   <sheets>
-    <sheet name="individual_services" sheetId="2" r:id="rId1"/>
-    <sheet name="Tables" sheetId="3" r:id="rId2"/>
+    <sheet name="community_activities" sheetId="4" r:id="rId1"/>
+    <sheet name="time_tracker" sheetId="5" r:id="rId2"/>
+    <sheet name="Tables" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,13 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="214">
   <si>
     <t>Hours</t>
-  </si>
-  <si>
-    <t>Name 
-(Last, First)</t>
   </si>
   <si>
     <t>Time Begun 
@@ -52,23 +49,7 @@
 (HH:MM)</t>
   </si>
   <si>
-    <t>Service
-(Select one)</t>
-  </si>
-  <si>
-    <t>Priority Area 
-(Select one)</t>
-  </si>
-  <si>
-    <t>Funding Source 
-(Select one)</t>
-  </si>
-  <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>I&amp;R?
-(Yes/No)</t>
   </si>
   <si>
     <t>Service</t>
@@ -289,16 +270,435 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Issue Area
+(Select one)</t>
+  </si>
+  <si>
+    <t>Projects 
+(Select one)</t>
+  </si>
+  <si>
+    <t>Service Program
+(Select one)</t>
+  </si>
+  <si>
+    <t>Issue Area</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>Other Supports</t>
+  </si>
+  <si>
+    <t>Recreation</t>
+  </si>
+  <si>
+    <t>Relocation</t>
+  </si>
+  <si>
+    <t>Resource Development</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Assistive Technology</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibility Buildings - Technical Assistance: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounting: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advocacy Education: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advocacy Employment: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advocacy General: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Advocacy Health Care: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advocacy Housing: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Advocacy Transportation: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT-Comm Ed and Public Info; Presentations AT: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT-Outreach: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIL/MRS Collaboration: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTS - Administrative: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTS - Outreach: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment Meetings in the Community: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment Presentations: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment Workshop: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executive Director Search: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Focus Groups: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Community Outreach: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Meetings in the Community: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Program Support: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health Care Collaboration: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health Care Consumer Outreach: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health Care Materials for the Community: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Barrier Busters Meeting: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Classes: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL Coordinated Funding Meeting: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL VA-DN/M Meeting: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Investing In Abilities Attending: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investing In Abilities Speaking: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT Support: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Weir Scholarship: </t>
+  </si>
+  <si>
+    <t>Legislative Luncheon: Lunch w/legislators</t>
+  </si>
+  <si>
+    <t>Legislative Visit: Visit from legislators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEW Workshop: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NetCIL Entry And Maintenance: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newsletter General/Advocacy/Youth: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFT Community Education: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFT DN/M Meeting: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFT Housing Coordinators Network Meeting: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFT Outreach to Nursing Home Residents: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFT Waiver Meeting: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OJE/OJT General Program Support: </t>
+  </si>
+  <si>
+    <t>Other - Bereavement: Time off for death of family member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other - Holiday: </t>
+  </si>
+  <si>
+    <t>Other - Paid Time Off: vacation/sick/personal time off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peer Mentor Training: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation Classes and Events: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation Event Planning: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation Meetings in the Community: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation Newsletter: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation Presentations: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recreation Promotion: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reporting for Federal/State/Grant Reports: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Advocacy: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Collaboration and Networking: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Outreach: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Technical Assistance: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource Dev. Collaboration: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource Dev. Community Meetings: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource Dev. Presentations in the Community: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource Dev. Volunteer Recruitment &amp; Mgmt: </t>
+  </si>
+  <si>
+    <t>RICC Meeting: Attendance at a RICC meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staff Educational Enrichment: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategic Planning: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Support Groups: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surveys General: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surveys Internal: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Meeting: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation - Collaboration: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation - Community Education: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation - Technical Assistance: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Way Homelessness Coalition: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website/Social Media: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Advocacy: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Collaboration: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Comm Ed And Public Info: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Event Marketing: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth IL Skills: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Recreation Events: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibility Programs - Technical Assistance: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curriculum Development: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAST Collaboration: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT-Technical Assistance: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefactor Development: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAST Marketing: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAST Presentations: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAW Marketing: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disability Awareness Workshops: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment Promotion: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFT Billing: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other - Inclement Weather: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Presentations and Community Education: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource Dev. Other/Internal: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Outreach: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Youth Volunteer Management: </t>
+  </si>
+  <si>
+    <t>Service Program</t>
+  </si>
+  <si>
+    <t>Collaboration/Networking</t>
+  </si>
+  <si>
+    <t>Community Education and Public Information</t>
+  </si>
+  <si>
+    <t>Community/Systems Advocacy</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Outreach Efforts</t>
+  </si>
+  <si>
+    <t>Technical Assistance</t>
+  </si>
+  <si>
+    <t>Funding Source
+(Select one)</t>
+  </si>
+  <si>
+    <t>Prjects-TT</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>CILs First Training/Entry/Maintenance</t>
+  </si>
+  <si>
+    <t>CTS - Administrative</t>
+  </si>
+  <si>
+    <t>General Program Support</t>
+  </si>
+  <si>
+    <t>Other - Holiday</t>
+  </si>
+  <si>
+    <t>Other - Inclement Weather</t>
+  </si>
+  <si>
+    <t>Other - Paid Time Off</t>
+  </si>
+  <si>
+    <t>Reporting for Federal/State/Local Grant Reports</t>
+  </si>
+  <si>
+    <t>Staff Meeting</t>
+  </si>
+  <si>
+    <t>Strategic Planning</t>
+  </si>
+  <si>
+    <t>Surveys Internal</t>
+  </si>
+  <si>
+    <t>Curriculum Development</t>
+  </si>
+  <si>
+    <t>Other - Bereavement</t>
+  </si>
+  <si>
+    <t>Team Meeting</t>
+  </si>
+  <si>
+    <t>Projects
+(Select one)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disability Network Meetings: </t>
+  </si>
+  <si>
+    <t>Time Begun 
+(HH:MM am/pm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +706,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF201F1E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,18 +743,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCFF"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -359,57 +792,241 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -462,6 +1079,46 @@
   <autoFilter ref="B34:B36" xr:uid="{7909C059-2AB2-4C4D-A56E-6361791DCC5D}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{4EBA9A07-62EF-416F-A801-06185FACC512}" name="IR"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{996F4033-A8C0-934B-B851-4DC8E8A8D300}" name="Table2" displayName="Table2" ref="F2:F13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="F2:F13" xr:uid="{996F4033-A8C0-934B-B851-4DC8E8A8D300}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{685C4D27-E508-694C-998C-9F9D8F0E56F9}" name="Issue Area" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8FC6E9E5-33AE-D34F-92F0-701A80D51DBA}" name="Table7" displayName="Table7" ref="B39:B45" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="B39:B45" xr:uid="{8FC6E9E5-33AE-D34F-92F0-701A80D51DBA}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{6F8A2B99-ECA7-484C-AC5D-071D1629D563}" name="Service Program" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B72C1162-7CAF-AC47-A252-2330AD13E89D}" name="Table8" displayName="Table8" ref="B47:B61" totalsRowShown="0">
+  <autoFilter ref="B47:B61" xr:uid="{B72C1162-7CAF-AC47-A252-2330AD13E89D}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{4C8A7377-AB11-1A43-AAC9-FEF5A6BAB2B3}" name="Prjects-TT"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{E9328D2C-74E4-F349-8745-D7FB8243105E}" name="Table510" displayName="Table510" ref="F16:F113" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="F16:F113" xr:uid="{E9328D2C-74E4-F349-8745-D7FB8243105E}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{3772237D-28E7-A347-8127-DB03C125E6D4}" name="Projects" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -763,98 +1420,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475C1560-65C8-49F6-9B9A-F6715764C657}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2BDEC6-2801-1D4A-9692-FAD438D7D05C}">
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1048548" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1048551" sqref="B1048551"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="13" style="11" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="46.83203125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9" style="5"/>
+    <col min="1" max="1" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="21"/>
+    <col min="3" max="3" width="16.1640625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="19.5" style="21" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="52.1640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="I15" s="8"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Spell check!" prompt="Please ensure both the last name and first name are spelled correctly and in the required format (Last, First)_x000a_" sqref="A2:A1048576" xr:uid="{C37A8EAA-4863-4C4F-9940-74929C156380}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tip" prompt="Hit alt + enter for a line break" sqref="I3:I1048576" xr:uid="{351EC2AD-ED4D-4752-A077-6F18AD5FC4B2}"/>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{11BCFCDE-454A-4642-B56C-EB4EAADF1EEE}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{FE2648CF-394D-0E42-92BF-0D11CC02D151}">
           <x14:formula1>
-            <xm:f>Tables!$B$3:$B$32</xm:f>
+            <xm:f>Tables!$F$3:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{EE005901-6FAD-9B4E-B3B3-69CAA3A67DEC}">
+          <x14:formula1>
+            <xm:f>Tables!$F$17:$F$112</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{4EF3F0E7-DE94-44DD-9B36-A7CBA395D4EB}">
-          <x14:formula1>
-            <xm:f>Tables!$D$3:$D$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{BC393DBA-6318-40FF-B771-4B498D55A2CC}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{9DA269C8-B031-1D4B-A2F3-D5C9AC9D8C1D}">
           <x14:formula1>
             <xm:f>Tables!$D$17:$D$42</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048547</xm:sqref>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{B9C4133B-93F9-49DC-B258-9A5C2DAF76DC}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{5BA01982-278D-E34C-9669-EF08160F8389}">
           <x14:formula1>
-            <xm:f>Tables!$B$35:$B$36</xm:f>
+            <xm:f>Tables!$B$40:$B$45</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Tip" prompt="Use &quot;Core&quot; unless otherwise specified_x000a__x000a_" xr:uid="{604FE682-7152-4EC2-8EED-7B71D9153FB4}">
-          <x14:formula1>
-            <xm:f>Tables!$D$17:$D$42</xm:f>
-          </x14:formula1>
-          <xm:sqref>H1048548:H1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -863,328 +1544,1029 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C89BC-5FF8-6A4C-8ECD-0972A33DF17A}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="16" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="19" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="54.1640625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="17">
+        <v>0.375</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="F22" s="14"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{5D823223-585F-574A-B10F-BB98531A55C1}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{5D516EF8-3756-0C46-BF03-6F475D72A247}">
+          <x14:formula1>
+            <xm:f>Tables!$B$48:$B$61</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07246D3C-C6EF-F446-8C8E-B742DA92975A}">
+          <x14:formula1>
+            <xm:f>Tables!$D$17:$D$42</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D25536F-9C4B-4B66-A9D8-B0C5C74E4EE3}">
-  <dimension ref="B2:D42"/>
+  <dimension ref="B2:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="F7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="F8" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="F9" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="F18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="F19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="F20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D21" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D22" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+      <c r="F22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+      <c r="F23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D24" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+      <c r="F24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="F25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>27</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D26" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+      <c r="F26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="F27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D28" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="F28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D29" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="F29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D30" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D31" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="F31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="F33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="F34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="F35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="F36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D33" t="s">
+      <c r="F37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="F38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="F39" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D40" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="F40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D37" t="s">
+      <c r="F41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D42" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D39" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
-        <v>78</v>
+      <c r="F42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>196</v>
+      </c>
+      <c r="F47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>197</v>
+      </c>
+      <c r="F48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>198</v>
+      </c>
+      <c r="F49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>199</v>
+      </c>
+      <c r="F50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>208</v>
+      </c>
+      <c r="F51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>200</v>
+      </c>
+      <c r="F52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>209</v>
+      </c>
+      <c r="F53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>201</v>
+      </c>
+      <c r="F54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>202</v>
+      </c>
+      <c r="F55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>203</v>
+      </c>
+      <c r="F56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>204</v>
+      </c>
+      <c r="F57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>205</v>
+      </c>
+      <c r="F58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>206</v>
+      </c>
+      <c r="F59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>207</v>
+      </c>
+      <c r="F60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>210</v>
+      </c>
+      <c r="F61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F71" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F73" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F74" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F75" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F77" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F78" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F79" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F81" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F82" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F83" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F84" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F86" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F87" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F88" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F89" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F90" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F91" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F92" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F93" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F94" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F95" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F96" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F97" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F98" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F99" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F100" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F101" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F102" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F103" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F104" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F105" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F106" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F107" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F108" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F109" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F110" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F111" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F112" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F113" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove time fix function. Input will be expected string
</commit_message>
<xml_diff>
--- a/reporting_template.xlsx
+++ b/reporting_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matte/Git/CILs-first-bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A671ED8F-63AE-024C-8AFA-F56A4E7E57C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB626EB-08A1-E646-9EBB-B886420F0AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="760" windowWidth="29180" windowHeight="18880" activeTab="1" xr2:uid="{F0BE1F58-B81B-4224-92BC-96133C095D6B}"/>
   </bookViews>
@@ -693,10 +693,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -796,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -841,16 +839,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -859,10 +848,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1423,20 +1415,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2BDEC6-2801-1D4A-9692-FAD438D7D05C}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="21"/>
-    <col min="3" max="3" width="16.1640625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="19.5" style="21" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="18"/>
+    <col min="3" max="3" width="16.1640625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="19.5" style="18" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="18" customWidth="1"/>
     <col min="9" max="9" width="52.1640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1470,8 +1462,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1548,16 +1540,16 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="16" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="19" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="19" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="16" customWidth="1"/>
     <col min="6" max="6" width="54.1640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1582,97 +1574,27 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="17">
-        <v>0.375</v>
-      </c>
-      <c r="C2" s="17"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-    </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F22" s="14"/>
     </row>
   </sheetData>
@@ -1693,7 +1615,7 @@
           <x14:formula1>
             <xm:f>Tables!$D$17:$D$42</xm:f>
           </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>